<commit_message>
Update report and values
</commit_message>
<xml_diff>
--- a/weekly/2025-CW09_weight_tracking.xlsx
+++ b/weekly/2025-CW09_weight_tracking.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,14 +586,38 @@
       <c r="B7" t="n">
         <v>98.2</v>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>98.8</v>
+      </c>
       <c r="D7" t="n">
         <v>28.7</v>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>27.7</v>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45946</v>
+      </c>
+      <c r="B8" t="n">
+        <v>98</v>
+      </c>
+      <c r="C8" t="n">
+        <v>98.09999999999999</v>
+      </c>
+      <c r="D8" t="n">
+        <v>28.6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>